<commit_message>
Passing all tests. Coverage at 80%
</commit_message>
<xml_diff>
--- a/test_constraints_w_errs.xlsx
+++ b/test_constraints_w_errs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HumeD\PycharmProjects\Data_Profile_Tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4893DBA0-3E34-46DB-9E9A-9E9E39D1A3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC45D79D-2157-40C8-9A06-A3A34C03D35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{D2E9D144-5D6F-4AC1-9DA3-D4FF634D9598}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2860" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2918" uniqueCount="206">
   <si>
     <t>Constraint_Set_Name</t>
   </si>
@@ -635,6 +635,30 @@
   </si>
   <si>
     <t>int,object,object,object,int,int,int</t>
+  </si>
+  <si>
+    <t>FAIL: Absolute Dimension Cross Product Element Row Count 1</t>
+  </si>
+  <si>
+    <t>FAIL: Absolute Dimension Cross Product Element Row Count 2</t>
+  </si>
+  <si>
+    <t>PASS: Absolute Dimension Cross Product Element Row Count</t>
+  </si>
+  <si>
+    <t>FAIL: Relative Dimension Cross Product Element Row Count 1</t>
+  </si>
+  <si>
+    <t>FAIL: Relative Dimension Cross Product Element Row Count 2</t>
+  </si>
+  <si>
+    <t>PASS: Relative Dimension Cross Product Element Row Count</t>
+  </si>
+  <si>
+    <t>FAIL: Relative Column Name</t>
+  </si>
+  <si>
+    <t>PASS: Relative Column Name</t>
   </si>
 </sst>
 </file>
@@ -692,7 +716,287 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="71">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1456,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E86614-3B97-43D1-B6C4-36CEB2305CDA}">
-  <dimension ref="A1:K400"/>
+  <dimension ref="A1:K408"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A391" workbookViewId="0">
+      <selection activeCell="B407" sqref="B407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15476,155 +15780,635 @@
         <v>1</v>
       </c>
     </row>
+    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A401" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B401">
+        <v>1</v>
+      </c>
+      <c r="C401" t="s">
+        <v>198</v>
+      </c>
+      <c r="D401" t="s">
+        <v>44</v>
+      </c>
+      <c r="E401" t="s">
+        <v>193</v>
+      </c>
+      <c r="F401" t="s">
+        <v>143</v>
+      </c>
+      <c r="G401" t="s">
+        <v>144</v>
+      </c>
+      <c r="H401" t="s">
+        <v>21</v>
+      </c>
+      <c r="I401">
+        <v>11</v>
+      </c>
+      <c r="J401">
+        <v>20</v>
+      </c>
+      <c r="K401">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A402" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B402">
+        <v>1</v>
+      </c>
+      <c r="C402" t="s">
+        <v>199</v>
+      </c>
+      <c r="D402" t="s">
+        <v>44</v>
+      </c>
+      <c r="E402" t="s">
+        <v>193</v>
+      </c>
+      <c r="F402" t="s">
+        <v>143</v>
+      </c>
+      <c r="G402" t="s">
+        <v>144</v>
+      </c>
+      <c r="H402" t="s">
+        <v>21</v>
+      </c>
+      <c r="I402">
+        <v>1</v>
+      </c>
+      <c r="J402">
+        <v>9</v>
+      </c>
+      <c r="K402">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A403" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B403">
+        <v>1</v>
+      </c>
+      <c r="C403" t="s">
+        <v>200</v>
+      </c>
+      <c r="D403" t="s">
+        <v>43</v>
+      </c>
+      <c r="E403" t="s">
+        <v>193</v>
+      </c>
+      <c r="F403" t="s">
+        <v>143</v>
+      </c>
+      <c r="G403" t="s">
+        <v>144</v>
+      </c>
+      <c r="H403" t="s">
+        <v>21</v>
+      </c>
+      <c r="I403">
+        <v>10</v>
+      </c>
+      <c r="J403">
+        <v>10</v>
+      </c>
+      <c r="K403">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A404" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B404">
+        <v>1</v>
+      </c>
+      <c r="C404" t="s">
+        <v>201</v>
+      </c>
+      <c r="D404" t="s">
+        <v>44</v>
+      </c>
+      <c r="E404" t="s">
+        <v>194</v>
+      </c>
+      <c r="F404" t="s">
+        <v>143</v>
+      </c>
+      <c r="G404" t="s">
+        <v>144</v>
+      </c>
+      <c r="H404" t="s">
+        <v>21</v>
+      </c>
+      <c r="I404">
+        <v>0</v>
+      </c>
+      <c r="J404">
+        <v>0.5</v>
+      </c>
+      <c r="K404">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A405" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B405">
+        <v>1</v>
+      </c>
+      <c r="C405" t="s">
+        <v>202</v>
+      </c>
+      <c r="D405" t="s">
+        <v>44</v>
+      </c>
+      <c r="E405" t="s">
+        <v>194</v>
+      </c>
+      <c r="F405" t="s">
+        <v>143</v>
+      </c>
+      <c r="G405" t="s">
+        <v>144</v>
+      </c>
+      <c r="H405" t="s">
+        <v>21</v>
+      </c>
+      <c r="I405">
+        <v>0.5</v>
+      </c>
+      <c r="J405">
+        <v>0.8</v>
+      </c>
+      <c r="K405">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="406" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A406" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B406">
+        <v>1</v>
+      </c>
+      <c r="C406" t="s">
+        <v>203</v>
+      </c>
+      <c r="D406" t="s">
+        <v>43</v>
+      </c>
+      <c r="E406" t="s">
+        <v>194</v>
+      </c>
+      <c r="F406" t="s">
+        <v>143</v>
+      </c>
+      <c r="G406" t="s">
+        <v>144</v>
+      </c>
+      <c r="H406" t="s">
+        <v>21</v>
+      </c>
+      <c r="I406">
+        <v>1</v>
+      </c>
+      <c r="J406">
+        <v>1</v>
+      </c>
+      <c r="K406">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="407" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A407" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B407">
+        <v>1</v>
+      </c>
+      <c r="C407" t="s">
+        <v>204</v>
+      </c>
+      <c r="D407" t="s">
+        <v>44</v>
+      </c>
+      <c r="E407" t="s">
+        <v>130</v>
+      </c>
+      <c r="F407" t="s">
+        <v>21</v>
+      </c>
+      <c r="G407" t="s">
+        <v>21</v>
+      </c>
+      <c r="H407">
+        <v>0</v>
+      </c>
+      <c r="I407" t="s">
+        <v>21</v>
+      </c>
+      <c r="J407" t="s">
+        <v>21</v>
+      </c>
+      <c r="K407">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A408" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B408">
+        <v>1</v>
+      </c>
+      <c r="C408" t="s">
+        <v>205</v>
+      </c>
+      <c r="D408" t="s">
+        <v>43</v>
+      </c>
+      <c r="E408" t="s">
+        <v>130</v>
+      </c>
+      <c r="F408" t="s">
+        <v>21</v>
+      </c>
+      <c r="G408" t="s">
+        <v>21</v>
+      </c>
+      <c r="H408">
+        <v>0</v>
+      </c>
+      <c r="I408" t="s">
+        <v>21</v>
+      </c>
+      <c r="J408" t="s">
+        <v>21</v>
+      </c>
+      <c r="K408">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C186:K186 A1:K1 J187:K187 K188:K190 C394:C398 C400 C391:F391 G392:G393 C187:H188 C190:F190 C189:G189 H189:H190 C191:K390 A2:B400 C2:K182">
-    <cfRule type="containsBlanks" dxfId="30" priority="31">
+    <cfRule type="containsBlanks" dxfId="70" priority="71">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C183:C185">
-    <cfRule type="containsBlanks" dxfId="29" priority="30">
+    <cfRule type="containsBlanks" dxfId="69" priority="70">
       <formula>LEN(TRIM(C183))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="containsBlanks" dxfId="28" priority="29">
+    <cfRule type="containsBlanks" dxfId="68" priority="69">
       <formula>LEN(TRIM(D183))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D184">
-    <cfRule type="containsBlanks" dxfId="27" priority="28">
+    <cfRule type="containsBlanks" dxfId="67" priority="68">
       <formula>LEN(TRIM(D184))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D185">
-    <cfRule type="containsBlanks" dxfId="26" priority="27">
+    <cfRule type="containsBlanks" dxfId="66" priority="67">
       <formula>LEN(TRIM(D185))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E183">
-    <cfRule type="containsBlanks" dxfId="25" priority="26">
+    <cfRule type="containsBlanks" dxfId="65" priority="66">
       <formula>LEN(TRIM(E183))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E184">
-    <cfRule type="containsBlanks" dxfId="24" priority="25">
+    <cfRule type="containsBlanks" dxfId="64" priority="65">
       <formula>LEN(TRIM(E184))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E185">
-    <cfRule type="containsBlanks" dxfId="23" priority="24">
+    <cfRule type="containsBlanks" dxfId="63" priority="64">
       <formula>LEN(TRIM(E185))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F183:K183">
-    <cfRule type="containsBlanks" dxfId="22" priority="23">
+    <cfRule type="containsBlanks" dxfId="62" priority="63">
       <formula>LEN(TRIM(F183))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F184:K184">
-    <cfRule type="containsBlanks" dxfId="21" priority="22">
+    <cfRule type="containsBlanks" dxfId="61" priority="62">
       <formula>LEN(TRIM(F184))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F185:K185">
-    <cfRule type="containsBlanks" dxfId="20" priority="21">
+    <cfRule type="containsBlanks" dxfId="60" priority="61">
       <formula>LEN(TRIM(F185))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I187">
-    <cfRule type="containsBlanks" dxfId="19" priority="20">
+    <cfRule type="containsBlanks" dxfId="59" priority="60">
       <formula>LEN(TRIM(I187))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I188">
-    <cfRule type="containsBlanks" dxfId="18" priority="19">
+    <cfRule type="containsBlanks" dxfId="58" priority="59">
       <formula>LEN(TRIM(I188))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J188">
-    <cfRule type="containsBlanks" dxfId="17" priority="18">
+    <cfRule type="containsBlanks" dxfId="57" priority="58">
       <formula>LEN(TRIM(J188))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J189">
-    <cfRule type="containsBlanks" dxfId="16" priority="17">
+    <cfRule type="containsBlanks" dxfId="56" priority="57">
       <formula>LEN(TRIM(J189))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I189">
-    <cfRule type="containsBlanks" dxfId="15" priority="16">
+    <cfRule type="containsBlanks" dxfId="55" priority="56">
       <formula>LEN(TRIM(I189))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I190">
-    <cfRule type="containsBlanks" dxfId="14" priority="15">
+    <cfRule type="containsBlanks" dxfId="54" priority="55">
       <formula>LEN(TRIM(I190))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J190">
-    <cfRule type="containsBlanks" dxfId="13" priority="14">
+    <cfRule type="containsBlanks" dxfId="53" priority="54">
       <formula>LEN(TRIM(J190))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C392">
-    <cfRule type="containsBlanks" dxfId="12" priority="13">
+    <cfRule type="containsBlanks" dxfId="52" priority="53">
       <formula>LEN(TRIM(C392))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C393">
-    <cfRule type="containsBlanks" dxfId="11" priority="12">
+    <cfRule type="containsBlanks" dxfId="51" priority="52">
       <formula>LEN(TRIM(C393))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C399">
-    <cfRule type="containsBlanks" dxfId="10" priority="10">
+    <cfRule type="containsBlanks" dxfId="50" priority="50">
       <formula>LEN(TRIM(C399))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D392:D398 D400">
-    <cfRule type="containsBlanks" dxfId="9" priority="9">
+    <cfRule type="containsBlanks" dxfId="49" priority="49">
       <formula>LEN(TRIM(D392))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D399">
-    <cfRule type="containsBlanks" dxfId="8" priority="8">
+    <cfRule type="containsBlanks" dxfId="48" priority="48">
       <formula>LEN(TRIM(D399))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E392:E400">
-    <cfRule type="containsBlanks" dxfId="7" priority="7">
+    <cfRule type="containsBlanks" dxfId="47" priority="47">
       <formula>LEN(TRIM(E392))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F392:F400">
-    <cfRule type="containsBlanks" dxfId="6" priority="6">
+    <cfRule type="containsBlanks" dxfId="46" priority="46">
       <formula>LEN(TRIM(F392))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G394:G400">
-    <cfRule type="containsBlanks" dxfId="5" priority="5">
+    <cfRule type="containsBlanks" dxfId="45" priority="45">
       <formula>LEN(TRIM(G394))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G391">
-    <cfRule type="containsBlanks" dxfId="4" priority="4">
+    <cfRule type="containsBlanks" dxfId="44" priority="44">
       <formula>LEN(TRIM(G391))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H393">
-    <cfRule type="containsBlanks" dxfId="3" priority="3">
+    <cfRule type="containsBlanks" dxfId="43" priority="43">
       <formula>LEN(TRIM(H393))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I391:K400">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
+    <cfRule type="containsBlanks" dxfId="42" priority="42">
       <formula>LEN(TRIM(I391))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G190">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="41" priority="41">
       <formula>LEN(TRIM(G190))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C403 C401:G401 K401:K406">
+    <cfRule type="containsBlanks" dxfId="39" priority="40">
+      <formula>LEN(TRIM(C401))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E402">
+    <cfRule type="containsBlanks" dxfId="38" priority="39">
+      <formula>LEN(TRIM(E402))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E403">
+    <cfRule type="containsBlanks" dxfId="37" priority="38">
+      <formula>LEN(TRIM(E403))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E404">
+    <cfRule type="containsBlanks" dxfId="36" priority="37">
+      <formula>LEN(TRIM(E404))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E405">
+    <cfRule type="containsBlanks" dxfId="35" priority="36">
+      <formula>LEN(TRIM(E405))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E406">
+    <cfRule type="containsBlanks" dxfId="34" priority="35">
+      <formula>LEN(TRIM(E406))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A401:B401">
+    <cfRule type="containsBlanks" dxfId="33" priority="34">
+      <formula>LEN(TRIM(A401))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A402:B402">
+    <cfRule type="containsBlanks" dxfId="32" priority="33">
+      <formula>LEN(TRIM(A402))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A403:B403">
+    <cfRule type="containsBlanks" dxfId="31" priority="32">
+      <formula>LEN(TRIM(A403))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A404:B404">
+    <cfRule type="containsBlanks" dxfId="30" priority="31">
+      <formula>LEN(TRIM(A404))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A405:B405">
+    <cfRule type="containsBlanks" dxfId="29" priority="30">
+      <formula>LEN(TRIM(A405))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A406:B406">
+    <cfRule type="containsBlanks" dxfId="28" priority="29">
+      <formula>LEN(TRIM(A406))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D402">
+    <cfRule type="containsBlanks" dxfId="27" priority="28">
+      <formula>LEN(TRIM(D402))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D404">
+    <cfRule type="containsBlanks" dxfId="26" priority="27">
+      <formula>LEN(TRIM(D404))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D405">
+    <cfRule type="containsBlanks" dxfId="25" priority="26">
+      <formula>LEN(TRIM(D405))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C402">
+    <cfRule type="containsBlanks" dxfId="24" priority="25">
+      <formula>LEN(TRIM(C402))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C404">
+    <cfRule type="containsBlanks" dxfId="23" priority="24">
+      <formula>LEN(TRIM(C404))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C405">
+    <cfRule type="containsBlanks" dxfId="22" priority="23">
+      <formula>LEN(TRIM(C405))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C406">
+    <cfRule type="containsBlanks" dxfId="21" priority="22">
+      <formula>LEN(TRIM(C406))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F402">
+    <cfRule type="containsBlanks" dxfId="20" priority="21">
+      <formula>LEN(TRIM(F402))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F403">
+    <cfRule type="containsBlanks" dxfId="19" priority="20">
+      <formula>LEN(TRIM(F403))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F404">
+    <cfRule type="containsBlanks" dxfId="18" priority="19">
+      <formula>LEN(TRIM(F404))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F405">
+    <cfRule type="containsBlanks" dxfId="17" priority="18">
+      <formula>LEN(TRIM(F405))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F406">
+    <cfRule type="containsBlanks" dxfId="16" priority="17">
+      <formula>LEN(TRIM(F406))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H401">
+    <cfRule type="containsBlanks" dxfId="15" priority="16">
+      <formula>LEN(TRIM(H401))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H402">
+    <cfRule type="containsBlanks" dxfId="14" priority="15">
+      <formula>LEN(TRIM(H402))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H403">
+    <cfRule type="containsBlanks" dxfId="13" priority="14">
+      <formula>LEN(TRIM(H403))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H404">
+    <cfRule type="containsBlanks" dxfId="12" priority="13">
+      <formula>LEN(TRIM(H404))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H405">
+    <cfRule type="containsBlanks" dxfId="11" priority="12">
+      <formula>LEN(TRIM(H405))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H406">
+    <cfRule type="containsBlanks" dxfId="10" priority="11">
+      <formula>LEN(TRIM(H406))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G402">
+    <cfRule type="containsBlanks" dxfId="9" priority="10">
+      <formula>LEN(TRIM(G402))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G403">
+    <cfRule type="containsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(G403))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G404">
+    <cfRule type="containsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(G404))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G405">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(G405))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G406">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(G406))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K407:K408">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(K407))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A407:B407">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A407))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A408:B408">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(A408))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C407">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(C407))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C408">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(C408))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15649,7 +16433,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I17">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="40" priority="1">
       <formula>LEN(TRIM(I17))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>